<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI5-Sandbox@dee937182dc83085911f07dbd4d083574306babd 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-encounter.xlsx
+++ b/StructureDefinition-us-core-encounter.xlsx
@@ -621,10 +621,10 @@
     <t>DomainResource.extension</t>
   </si>
   <si>
-    <t>Encounter.extension:us-core-interpreter-required</t>
-  </si>
-  <si>
-    <t>us-core-interpreter-required</t>
+    <t>Encounter.extension:interpreterRequired</t>
+  </si>
+  <si>
+    <t>interpreterRequired</t>
   </si>
   <si>
     <t xml:space="preserve">Extension {http://hl7.org/fhir/us/uscdi5-sandbox/StructureDefinition/us-core-interpreter-required}
@@ -2105,9 +2105,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="46.3828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="45.67578125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="45.67578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="26.8359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="3" max="3" width="19.24609375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="4.9453125" customWidth="true" bestFit="true"/>

</xml_diff>